<commit_message>
Added LCSC number for 557nm and 496nm 3V3 0603 designs.
</commit_message>
<xml_diff>
--- a/3V3_0603/496nm/BOM_JLCPCB_496nm.xlsx
+++ b/3V3_0603/496nm/BOM_JLCPCB_496nm.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">D1</t>
   </si>
   <si>
-    <t xml:space="preserve">Global Parts</t>
+    <t xml:space="preserve">C2846641</t>
   </si>
 </sst>
 </file>
@@ -346,7 +346,7 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>